<commit_message>
Added Iridium 7 & 8
</commit_message>
<xml_diff>
--- a/Iridium NEXT 8/Excel/analysed.xlsx
+++ b/Iridium NEXT 8/Excel/analysed.xlsx
@@ -5214,7 +5214,7 @@
         <v>800.696</v>
       </c>
       <c r="E124" t="n">
-        <v>861.818</v>
+        <v>861.817</v>
       </c>
       <c r="F124" t="n">
         <v>28.341</v>
@@ -5359,7 +5359,7 @@
         <v>833.461</v>
       </c>
       <c r="E129" t="n">
-        <v>983.001</v>
+        <v>983.002</v>
       </c>
       <c r="F129" t="n">
         <v>29.275</v>
@@ -5388,7 +5388,7 @@
         <v>834.245</v>
       </c>
       <c r="E130" t="n">
-        <v>1010.47</v>
+        <v>1010.471</v>
       </c>
       <c r="F130" t="n">
         <v>29.261</v>
@@ -5414,10 +5414,10 @@
         <v>48.95</v>
       </c>
       <c r="D131" t="n">
-        <v>836.34</v>
+        <v>836.3390000000001</v>
       </c>
       <c r="E131" t="n">
-        <v>1037.957</v>
+        <v>1037.958</v>
       </c>
       <c r="F131" t="n">
         <v>29.325</v>
@@ -5443,10 +5443,10 @@
         <v>49.821</v>
       </c>
       <c r="D132" t="n">
-        <v>839.872</v>
+        <v>839.871</v>
       </c>
       <c r="E132" t="n">
-        <v>1064.889</v>
+        <v>1064.89</v>
       </c>
       <c r="F132" t="n">
         <v>29.507</v>
@@ -5472,10 +5472,10 @@
         <v>50.584</v>
       </c>
       <c r="D133" t="n">
-        <v>845.386</v>
+        <v>845.384</v>
       </c>
       <c r="E133" t="n">
-        <v>1091.249</v>
+        <v>1091.251</v>
       </c>
       <c r="F133" t="n">
         <v>29.928</v>
@@ -5501,13 +5501,13 @@
         <v>51.483</v>
       </c>
       <c r="D134" t="n">
-        <v>854.023</v>
+        <v>854.02</v>
       </c>
       <c r="E134" t="n">
-        <v>1116.901</v>
+        <v>1116.903</v>
       </c>
       <c r="F134" t="n">
-        <v>30.436</v>
+        <v>30.435</v>
       </c>
       <c r="G134" t="n">
         <v>36.454</v>
@@ -5530,10 +5530,10 @@
         <v>52.381</v>
       </c>
       <c r="D135" t="n">
-        <v>863.697</v>
+        <v>863.6950000000001</v>
       </c>
       <c r="E135" t="n">
-        <v>1142.104</v>
+        <v>1142.105</v>
       </c>
       <c r="F135" t="n">
         <v>31.049</v>
@@ -5559,10 +5559,10 @@
         <v>53.25</v>
       </c>
       <c r="D136" t="n">
-        <v>874.091</v>
+        <v>874.0890000000001</v>
       </c>
       <c r="E136" t="n">
-        <v>1167.086</v>
+        <v>1167.087</v>
       </c>
       <c r="F136" t="n">
         <v>31.582</v>
@@ -5588,10 +5588,10 @@
         <v>54.05</v>
       </c>
       <c r="D137" t="n">
-        <v>884.544</v>
+        <v>884.543</v>
       </c>
       <c r="E137" t="n">
-        <v>1192.263</v>
+        <v>1192.264</v>
       </c>
       <c r="F137" t="n">
         <v>32.061</v>
@@ -5620,7 +5620,7 @@
         <v>895.289</v>
       </c>
       <c r="E138" t="n">
-        <v>1217.854</v>
+        <v>1217.855</v>
       </c>
       <c r="F138" t="n">
         <v>32.484</v>
@@ -8729,7 +8729,7 @@
         <v>-0.027</v>
       </c>
       <c r="G245" t="n">
-        <v>154.718</v>
+        <v>154.719</v>
       </c>
       <c r="H245" t="n">
         <v>-13.617</v>
@@ -11919,7 +11919,7 @@
         <v>-17.238</v>
       </c>
       <c r="G355" t="n">
-        <v>230.078</v>
+        <v>230.079</v>
       </c>
       <c r="H355" t="n">
         <v>-57.744</v>
@@ -12644,7 +12644,7 @@
         <v>-29.583</v>
       </c>
       <c r="G380" t="n">
-        <v>240.702</v>
+        <v>240.703</v>
       </c>
       <c r="H380" t="n">
         <v>-59.059</v>

</xml_diff>